<commit_message>
The 'Functional Requirements' section has been modified in the ' TAWA_SoftwareRequirementSpecification_V1.0' document and 'TAWA_SystemRequirements'document has been modified
</commit_message>
<xml_diff>
--- a/TAWA_SystemRequirements.xlsx
+++ b/TAWA_SystemRequirements.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -178,13 +178,37 @@
     <t>The user will be able to book for his/her travel either going or going&amp;coming back trip.</t>
   </si>
   <si>
-    <t>The admin can add or delete users.</t>
-  </si>
-  <si>
     <t>The response time  of the website will be five seconds.</t>
   </si>
   <si>
     <t>The throughput of the website is 1000 request.</t>
+  </si>
+  <si>
+    <t>The admin can add, search and delete users.</t>
+  </si>
+  <si>
+    <t>SR_014</t>
+  </si>
+  <si>
+    <t>The user will be able to see Travel destination details.</t>
+  </si>
+  <si>
+    <t>The user will be able to Explore Different Airlines.</t>
+  </si>
+  <si>
+    <t>SR_015</t>
+  </si>
+  <si>
+    <t>The user will be able to Send Feedback and share his experiences.</t>
+  </si>
+  <si>
+    <t>SR_016</t>
+  </si>
+  <si>
+    <t>The user and the admin will be able to logout.</t>
+  </si>
+  <si>
+    <t>SR_017</t>
   </si>
 </sst>
 </file>
@@ -243,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -292,11 +316,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -321,6 +356,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -627,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -702,7 +740,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -722,7 +760,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -742,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -762,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -782,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -843,47 +881,49 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
     </row>
     <row r="12" spans="1:15" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>26</v>
+      <c r="B12" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
     </row>
     <row r="13" spans="1:15" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -902,8 +942,8 @@
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>27</v>
+      <c r="B14" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -923,7 +963,7 @@
         <v>19</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -938,9 +978,13 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
     </row>
-    <row r="16" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:15" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -954,9 +998,13 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="1"/>
+    <row r="17" spans="1:14" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>26</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -970,9 +1018,13 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
     </row>
-    <row r="18" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="1"/>
+    <row r="18" spans="1:14" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -986,9 +1038,13 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="1"/>
+    <row r="19" spans="1:14" ht="18" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>35</v>
+      </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1197,22 +1253,70 @@
     <row r="32" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A32" s="6"/>
       <c r="B32" s="1"/>
-    </row>
-    <row r="33" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="6"/>
       <c r="B33" s="1"/>
-    </row>
-    <row r="34" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A34" s="6"/>
       <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A35" s="6"/>
       <c r="B35" s="1"/>
     </row>
-    <row r="36" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="18" x14ac:dyDescent="0.35">
       <c r="A36" s="6"/>
       <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A37" s="6"/>
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A38" s="6"/>
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:14" ht="18" x14ac:dyDescent="0.35">
+      <c r="A39" s="6"/>
+      <c r="B39" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>